<commit_message>
update file template sap
</commit_message>
<xml_diff>
--- a/public/excel/SapMaterial.xlsx
+++ b/public/excel/SapMaterial.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Mã SAP</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>KG</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +395,7 @@
     <col min="7" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +405,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40001374</v>
       </c>

</xml_diff>